<commit_message>
Primer backup local de Mio Fratello
</commit_message>
<xml_diff>
--- a/public/templates/Bulk_Product_Upload_Template.xlsx
+++ b/public/templates/Bulk_Product_Upload_Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>opening_stock</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>alert_quantity</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,44 +363,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A2:H3"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="5" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="31.85546875" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>